<commit_message>
Lo mejor es no pensarlo peña
</commit_message>
<xml_diff>
--- a/Actividad3/Segunda hoja.xlsx
+++ b/Actividad3/Segunda hoja.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a8f7cf7c30acf5e3/Documentos/GitHub/PythonDataScience_Group_Project/Actividad3/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Angel\Documents\GitHub\PythonDataScience_Group_Project\Actividad3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="8_{4470D6EA-FE8B-4CCF-B32C-D91B4F94B176}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E9BEC98B-454C-4ECB-B0C0-8E21BD9B086C}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{168ADCD3-A46E-4FB6-8D6B-D95B8D5EE69D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{0D3F3CCC-63B2-4EB8-9440-919B734BE40A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{0D3F3CCC-63B2-4EB8-9440-919B734BE40A}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="8">
   <si>
     <t>Nombre</t>
   </si>
@@ -610,10 +610,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -993,7 +989,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{124ED1F1-82B4-487D-8B06-3A3EDCDE46A4}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
@@ -1049,28 +1045,14 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFB148C2-B075-4023-A735-055928ABF6F9}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A2:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-    </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
@@ -1082,6 +1064,20 @@
         <v>5</v>
       </c>
       <c r="D2">
+        <v>2006</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3">
+        <v>339</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3">
         <v>2006</v>
       </c>
     </row>

</xml_diff>